<commit_message>
change to 4 carriers only
</commit_message>
<xml_diff>
--- a/config/jspecs - carrier.xlsx
+++ b/config/jspecs - carrier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\p3388_general_rfi_tv\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D772F509-561D-4FB7-93B5-721FD5672E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CAD9C4-DA6D-4833-9969-A1709428DE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -425,7 +425,7 @@
   <dimension ref="A1:O183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -536,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>90</v>
+        <v>600</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -630,7 +630,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>130</v>
+        <v>800</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -670,12 +670,51 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="2">
+        <v>12</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>

</xml_diff>